<commit_message>
working 2v3c case and WIP 5v2c case
</commit_message>
<xml_diff>
--- a/assets/rapporto cilindri viste.xlsx
+++ b/assets/rapporto cilindri viste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enric\Documents\GitHub\Geometric-Aware-Camera-Pose-Estimation\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C017A8F2-BDCF-4C97-AA02-6D4219080944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDAF670-283D-4FE9-B8C4-92472CED7469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{C36F357A-DAD5-41FF-9C2E-E2ABE59EE17D}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -112,49 +112,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1331,7 +1289,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,7 +1620,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2004,27 +1962,27 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <f>CEILING(B$1/(2*$A14-3),1)</f>
+        <f t="shared" ref="B14:G23" si="10">CEILING(B$1/(2*$A14-3),1)</f>
         <v>0</v>
       </c>
       <c r="C14">
-        <f>CEILING(C$1/(2*$A14-3),1)</f>
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
       <c r="D14">
-        <f>CEILING(D$1/(2*$A14-3),1)</f>
+        <f t="shared" si="10"/>
         <v>-2</v>
       </c>
       <c r="E14">
-        <f>CEILING(E$1/(2*$A14-3),1)</f>
+        <f t="shared" si="10"/>
         <v>-3</v>
       </c>
       <c r="F14">
-        <f>CEILING(F$1/(2*$A14-3),1)</f>
+        <f t="shared" si="10"/>
         <v>-4</v>
       </c>
       <c r="G14">
-        <f>CEILING(G$1/(2*$A14-3),1)</f>
+        <f t="shared" si="10"/>
         <v>-5</v>
       </c>
     </row>
@@ -2033,27 +1991,27 @@
         <v>2</v>
       </c>
       <c r="B15">
-        <f>CEILING(B$1/(2*$A15-3),1)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C15">
-        <f>CEILING(C$1/(2*$A15-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="D15">
-        <f>CEILING(D$1/(2*$A15-3),1)</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="E15">
-        <f>CEILING(E$1/(2*$A15-3),1)</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="F15">
-        <f>CEILING(F$1/(2*$A15-3),1)</f>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="G15">
-        <f>CEILING(G$1/(2*$A15-3),1)</f>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
     </row>
@@ -2062,27 +2020,27 @@
         <v>3</v>
       </c>
       <c r="B16">
-        <f>CEILING(B$1/(2*$A16-3),1)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C16">
-        <f>CEILING(C$1/(2*$A16-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="D16">
-        <f>CEILING(D$1/(2*$A16-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="E16">
-        <f>CEILING(E$1/(2*$A16-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="F16">
-        <f>CEILING(F$1/(2*$A16-3),1)</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="G16">
-        <f>CEILING(G$1/(2*$A16-3),1)</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
     </row>
@@ -2091,27 +2049,27 @@
         <v>4</v>
       </c>
       <c r="B17">
-        <f>CEILING(B$1/(2*$A17-3),1)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C17">
-        <f>CEILING(C$1/(2*$A17-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="D17">
-        <f>CEILING(D$1/(2*$A17-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="E17">
-        <f>CEILING(E$1/(2*$A17-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="F17">
-        <f>CEILING(F$1/(2*$A17-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G17">
-        <f>CEILING(G$1/(2*$A17-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
@@ -2120,27 +2078,27 @@
         <v>5</v>
       </c>
       <c r="B18">
-        <f>CEILING(B$1/(2*$A18-3),1)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C18">
-        <f>CEILING(C$1/(2*$A18-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="D18">
-        <f>CEILING(D$1/(2*$A18-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="E18">
-        <f>CEILING(E$1/(2*$A18-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="F18">
-        <f>CEILING(F$1/(2*$A18-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G18">
-        <f>CEILING(G$1/(2*$A18-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
@@ -2149,27 +2107,27 @@
         <v>6</v>
       </c>
       <c r="B19">
-        <f>CEILING(B$1/(2*$A19-3),1)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C19">
-        <f>CEILING(C$1/(2*$A19-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="D19">
-        <f>CEILING(D$1/(2*$A19-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="E19">
-        <f>CEILING(E$1/(2*$A19-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="F19">
-        <f>CEILING(F$1/(2*$A19-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G19">
-        <f>CEILING(G$1/(2*$A19-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
@@ -2178,27 +2136,27 @@
         <v>7</v>
       </c>
       <c r="B20">
-        <f>CEILING(B$1/(2*$A20-3),1)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C20">
-        <f>CEILING(C$1/(2*$A20-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="D20">
-        <f>CEILING(D$1/(2*$A20-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="E20">
-        <f>CEILING(E$1/(2*$A20-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="F20">
-        <f>CEILING(F$1/(2*$A20-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G20">
-        <f>CEILING(G$1/(2*$A20-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
@@ -2207,27 +2165,27 @@
         <v>8</v>
       </c>
       <c r="B21">
-        <f>CEILING(B$1/(2*$A21-3),1)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C21">
-        <f>CEILING(C$1/(2*$A21-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="D21">
-        <f>CEILING(D$1/(2*$A21-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="E21">
-        <f>CEILING(E$1/(2*$A21-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="F21">
-        <f>CEILING(F$1/(2*$A21-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G21">
-        <f>CEILING(G$1/(2*$A21-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
@@ -2236,27 +2194,27 @@
         <v>9</v>
       </c>
       <c r="B22">
-        <f>CEILING(B$1/(2*$A22-3),1)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C22">
-        <f>CEILING(C$1/(2*$A22-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="D22">
-        <f>CEILING(D$1/(2*$A22-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="E22">
-        <f>CEILING(E$1/(2*$A22-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="F22">
-        <f>CEILING(F$1/(2*$A22-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G22">
-        <f>CEILING(G$1/(2*$A22-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
@@ -2265,27 +2223,27 @@
         <v>10</v>
       </c>
       <c r="B23">
-        <f>CEILING(B$1/(2*$A23-3),1)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C23">
-        <f>CEILING(C$1/(2*$A23-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="D23">
-        <f>CEILING(D$1/(2*$A23-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="E23">
-        <f>CEILING(E$1/(2*$A23-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="F23">
-        <f>CEILING(F$1/(2*$A23-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G23">
-        <f>CEILING(G$1/(2*$A23-3),1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>